<commit_message>
Atualiza dados - 18/02/2026 10:01
</commit_message>
<xml_diff>
--- a/public/dados.xlsx
+++ b/public/dados.xlsx
@@ -8767,13 +8767,13 @@
         <v>12:00</v>
       </c>
       <c r="J220" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K220">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="L220" t="str">
-        <v>+2h</v>
+        <v>+0min</v>
       </c>
     </row>
     <row r="221">
@@ -15873,13 +15873,13 @@
         <v>12:03</v>
       </c>
       <c r="J407" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K407">
-        <v>418</v>
+        <v>3</v>
       </c>
       <c r="L407" t="str">
-        <v>+6h58min</v>
+        <v>+3min</v>
       </c>
     </row>
     <row r="408">
@@ -16101,13 +16101,13 @@
         <v>12:01</v>
       </c>
       <c r="J413" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K413">
-        <v>203</v>
+        <v>2</v>
       </c>
       <c r="L413" t="str">
-        <v>+3h23min</v>
+        <v>+2min</v>
       </c>
     </row>
     <row r="414">
@@ -41485,13 +41485,13 @@
         <v>12:09</v>
       </c>
       <c r="J1081" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K1081">
-        <v>251</v>
+        <v>10</v>
       </c>
       <c r="L1081" t="str">
-        <v>+4h11min</v>
+        <v>+10min</v>
       </c>
     </row>
     <row r="1082">
@@ -44145,13 +44145,13 @@
         <v>12:09</v>
       </c>
       <c r="J1151" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K1151">
-        <v>229</v>
+        <v>-1</v>
       </c>
       <c r="L1151" t="str">
-        <v>+3h49min</v>
+        <v>-1min</v>
       </c>
     </row>
     <row r="1152">
@@ -45706,10 +45706,10 @@
         <v>Hora Extra</v>
       </c>
       <c r="K1192">
-        <v>262</v>
+        <v>29</v>
       </c>
       <c r="L1192" t="str">
-        <v>+4h22min</v>
+        <v>+29min</v>
       </c>
     </row>
     <row r="1193">
@@ -47071,13 +47071,13 @@
         <v>12:22</v>
       </c>
       <c r="J1228" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K1228">
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="L1228" t="str">
-        <v>+4h2min</v>
+        <v>+0min</v>
       </c>
     </row>
     <row r="1229">
@@ -52394,10 +52394,10 @@
         <v>Hora Extra</v>
       </c>
       <c r="K1368">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="L1368" t="str">
-        <v>+3h28min</v>
+        <v>+2h3min</v>
       </c>
     </row>
     <row r="1369">
@@ -53648,10 +53648,10 @@
         <v>Hora Extra</v>
       </c>
       <c r="K1401">
-        <v>206</v>
+        <v>120</v>
       </c>
       <c r="L1401" t="str">
-        <v>+3h26min</v>
+        <v>+2h</v>
       </c>
     </row>
     <row r="1402">
@@ -60067,13 +60067,13 @@
         <v>12:15</v>
       </c>
       <c r="J1570" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K1570">
-        <v>397</v>
+        <v>3</v>
       </c>
       <c r="L1570" t="str">
-        <v>+6h37min</v>
+        <v>+3min</v>
       </c>
     </row>
     <row r="1571">
@@ -64513,13 +64513,13 @@
         <v>12:00</v>
       </c>
       <c r="J1687" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K1687">
-        <v>524</v>
+        <v>-6</v>
       </c>
       <c r="L1687" t="str">
-        <v>+8h44min</v>
+        <v>-6min</v>
       </c>
     </row>
     <row r="1688">
@@ -67553,13 +67553,13 @@
         <v>12:00</v>
       </c>
       <c r="J1767" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K1767">
-        <v>527</v>
+        <v>-2</v>
       </c>
       <c r="L1767" t="str">
-        <v>+8h47min</v>
+        <v>-2min</v>
       </c>
     </row>
     <row r="1768">
@@ -77965,13 +77965,13 @@
         <v>12:01</v>
       </c>
       <c r="J2041" t="str">
-        <v>Hora Extra</v>
+        <v>Normal</v>
       </c>
       <c r="K2041">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="L2041" t="str">
-        <v>+2h30min</v>
+        <v>+1min</v>
       </c>
     </row>
     <row r="2042">
@@ -79979,13 +79979,13 @@
         <v>10:00</v>
       </c>
       <c r="J2094" t="str">
-        <v>Hora Extra</v>
+        <v>Atraso</v>
       </c>
       <c r="K2094">
-        <v>89</v>
+        <v>-120</v>
       </c>
       <c r="L2094" t="str">
-        <v>+1h29min</v>
+        <v>-2h</v>
       </c>
     </row>
     <row r="2095">

</xml_diff>